<commit_message>
documentatio: Add documentation from google Drive
</commit_message>
<xml_diff>
--- a/Documentation/Unit Tests/MVP/TestCases.xlsx
+++ b/Documentation/Unit Tests/MVP/TestCases.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="133">
   <si>
     <t>ID</t>
   </si>
@@ -52,54 +52,84 @@
     <t>Verify successful login with correct username and password combination</t>
   </si>
   <si>
+    <t>Successful login</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>IT1-1 TC2</t>
+  </si>
+  <si>
+    <t>Invalid Password entered</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ensure appropriate error message is displayed when an incorrect password is entered</t>
+  </si>
+  <si>
+    <t>Error message is displayed when an incorrect password is entered</t>
+  </si>
+  <si>
+    <t>IT1-1 TC3</t>
+  </si>
+  <si>
+    <t>Blank spaces</t>
+  </si>
+  <si>
+    <t>Confirm that an error message is displayed and the user can not enter to the system</t>
+  </si>
+  <si>
+    <t>Error message is displayed and the user can not enter to the system</t>
+  </si>
+  <si>
+    <t>IT1-2</t>
+  </si>
+  <si>
+    <t>Create product</t>
+  </si>
+  <si>
+    <t>IT1-2 TC1</t>
+  </si>
+  <si>
+    <t>Successful Product Creation</t>
+  </si>
+  <si>
+    <t>Verify that a new product is created successfully with valid input</t>
+  </si>
+  <si>
+    <t>created successfully with valid input</t>
+  </si>
+  <si>
+    <t>IT1-2 TC2</t>
+  </si>
+  <si>
+    <t>Required Fields</t>
+  </si>
+  <si>
+    <t>Validate that appropriate error messages are displayed when required fields are left blank</t>
+  </si>
+  <si>
+    <t>error messages are displayed when required fields are left blank</t>
+  </si>
+  <si>
+    <t>IT1-2 TC3</t>
+  </si>
+  <si>
+    <t>Duplicate Product</t>
+  </si>
+  <si>
+    <t>Ensure that a proper error message is shown when attempting to create a product with an existing name or identifier</t>
+  </si>
+  <si>
+    <t>error message is shown when attempting to create a product with an existing name or identifier</t>
+  </si>
+  <si>
+    <t>IT1-2 TC4</t>
+  </si>
+  <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>IT1-1 TC2</t>
-  </si>
-  <si>
-    <t>Invalid Password entered</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ensure appropriate error message is displayed when an incorrect password is entered</t>
-  </si>
-  <si>
-    <t>IT1-1 TC3</t>
-  </si>
-  <si>
-    <t>Account Lockout</t>
-  </si>
-  <si>
-    <t>Confirm user is locked out after a specified number of failed login attempts</t>
-  </si>
-  <si>
-    <t>IT1-1 TC4</t>
-  </si>
-  <si>
-    <t>Forgot Password</t>
-  </si>
-  <si>
-    <t>Test the password recovery functionality and validate successful password reset process</t>
-  </si>
-  <si>
-    <t>IT1-2</t>
-  </si>
-  <si>
-    <t>Create product</t>
-  </si>
-  <si>
-    <t>IT1-2 TC1</t>
-  </si>
-  <si>
-    <t>IT1-2 TC2</t>
-  </si>
-  <si>
-    <t>IT1-2 TC3</t>
-  </si>
-  <si>
-    <t>IT1-2 TC4</t>
-  </si>
-  <si>
     <t>IT1-3</t>
   </si>
   <si>
@@ -109,13 +139,13 @@
     <t>IT1-3 TC1</t>
   </si>
   <si>
-    <t>IT1-3 TC2</t>
-  </si>
-  <si>
-    <t>IT1-3 TC3</t>
-  </si>
-  <si>
-    <t>IT1-3 TC4</t>
+    <t>Successful Product Display</t>
+  </si>
+  <si>
+    <t>Verify that all products are displayed correctly without any missing or incorrect information.</t>
+  </si>
+  <si>
+    <t>All products are displayed correctly without any missing or incorrect information.</t>
   </si>
   <si>
     <t>IT1-4</t>
@@ -127,13 +157,37 @@
     <t>IT1-4 TC1</t>
   </si>
   <si>
+    <t>Product Details</t>
+  </si>
+  <si>
+    <t>Verify that all specifications and details of the specific product are accurately displayed</t>
+  </si>
+  <si>
+    <t>All specifications and details of the specific product are accurately displayed</t>
+  </si>
+  <si>
     <t>IT1-4 TC2</t>
   </si>
   <si>
+    <t>Images</t>
+  </si>
+  <si>
+    <t>Ensure that product images are properly displayed and accessible for viewing</t>
+  </si>
+  <si>
+    <t>Product images are properly displayed and accessible for viewing</t>
+  </si>
+  <si>
     <t>IT1-4 TC3</t>
   </si>
   <si>
-    <t>IT1-4 TC4</t>
+    <t xml:space="preserve">Pricing </t>
+  </si>
+  <si>
+    <t>Validate that pricing information of the product are accurately presented</t>
+  </si>
+  <si>
+    <t>Pricing information of the product are accurately presented</t>
   </si>
   <si>
     <t>IT1-5</t>
@@ -151,6 +205,9 @@
     <t>Verify that an admin account is successfully created with valid credentials</t>
   </si>
   <si>
+    <t>The admin user created has an encrypted password and can log in without problem as administrator:</t>
+  </si>
+  <si>
     <t>IT1-5 TC2</t>
   </si>
   <si>
@@ -160,6 +217,9 @@
     <t>Ensure that an error message is displayed when attempting to create an admin with an existing username</t>
   </si>
   <si>
+    <t>Error message is displayed when attempting to create an admin with an existing username</t>
+  </si>
+  <si>
     <t>IT1-5 TC3</t>
   </si>
   <si>
@@ -169,6 +229,9 @@
     <t>Validate that an error message is shown when providing an invalid email format during admin creation</t>
   </si>
   <si>
+    <t>Error message is shown when providing an invalid email format during admin creation</t>
+  </si>
+  <si>
     <t>IT1-5 TC4</t>
   </si>
   <si>
@@ -178,6 +241,9 @@
     <t>Test the system's response when attempting to create an admin account with a weak or easily guessable password</t>
   </si>
   <si>
+    <t xml:space="preserve">Error message with the note that the password is not strong </t>
+  </si>
+  <si>
     <t>IT1-5 TC5</t>
   </si>
   <si>
@@ -187,22 +253,25 @@
     <t>Validate that appropriate error messages are displayed when attempting to create an admin account with empty required fields</t>
   </si>
   <si>
+    <t>Error messages are displayed when attempting to create an admin account with empty required fields</t>
+  </si>
+  <si>
     <t>IT1-6</t>
   </si>
   <si>
-    <t>Browse report</t>
+    <t>Browse reports</t>
   </si>
   <si>
     <t>IT6- 1 TC1</t>
   </si>
   <si>
-    <t>IT6- 1 TC2</t>
-  </si>
-  <si>
-    <t>IT6- 1 TC3</t>
-  </si>
-  <si>
-    <t>IT6- 1 TC4</t>
+    <t>Successful Reports Display</t>
+  </si>
+  <si>
+    <t>Verify that all reports are displayed correctly without any missing or incorrect information.</t>
+  </si>
+  <si>
+    <t>All reports are displayed correctly without any missing or incorrect information.</t>
   </si>
   <si>
     <t>IT1-7</t>
@@ -214,13 +283,13 @@
     <t>IT1-7 TC1</t>
   </si>
   <si>
-    <t>IT1-7 TC2</t>
-  </si>
-  <si>
-    <t>IT1-7 TC3</t>
-  </si>
-  <si>
-    <t>IT1-7 TC4</t>
+    <t>Successful Logout</t>
+  </si>
+  <si>
+    <t>Verify that the user is successfully logged out of the system</t>
+  </si>
+  <si>
+    <t>User is successfully logged out of the system</t>
   </si>
   <si>
     <t>IT1-8</t>
@@ -232,49 +301,46 @@
     <t>IT1-8 TC1</t>
   </si>
   <si>
-    <t>IT1-8 TC2</t>
-  </si>
-  <si>
-    <t>IT1-8 TC3</t>
-  </si>
-  <si>
-    <t>IT1-8 TC4</t>
+    <t>Successful Product Deletion</t>
+  </si>
+  <si>
+    <t>Verify that the selected product is successfully deleted from the system</t>
+  </si>
+  <si>
+    <t>successfully deleted from the system</t>
   </si>
   <si>
     <t>IT1-9</t>
   </si>
   <si>
-    <t>Browse admin</t>
+    <t>Browse admins</t>
   </si>
   <si>
     <t>IT1-9 TC1</t>
   </si>
   <si>
-    <t>IT1-9 TC2</t>
-  </si>
-  <si>
-    <t>IT1-9 TC3</t>
-  </si>
-  <si>
-    <t>IT1-9 TC4</t>
+    <t>Successful admins Display</t>
+  </si>
+  <si>
+    <t>Verify that all admins are displayed correctly without any missing or incorrect information.</t>
+  </si>
+  <si>
+    <t>all admins are displayed correctly without any missing or incorrect information.</t>
   </si>
   <si>
     <t>IT1-10</t>
   </si>
   <si>
-    <t>Detete admin</t>
+    <t>Delete admin</t>
   </si>
   <si>
     <t>IT1-10 TC1</t>
   </si>
   <si>
-    <t>IT1-10 TC2</t>
-  </si>
-  <si>
-    <t>IT1-10 TC3</t>
-  </si>
-  <si>
-    <t>IT1-10 TC4</t>
+    <t>Successful admin Deletion</t>
+  </si>
+  <si>
+    <t>Verify that the selected admin is successfully deleted from the system</t>
   </si>
   <si>
     <t>IT1-11</t>
@@ -286,13 +352,28 @@
     <t>IT1-11 TC1</t>
   </si>
   <si>
+    <t>Successful Product Update</t>
+  </si>
+  <si>
+    <t>Verify that the selected product is successfully updated with valid input.</t>
+  </si>
+  <si>
+    <t>successfully updated with valid input.</t>
+  </si>
+  <si>
     <t>IT1-11 TC2</t>
   </si>
   <si>
-    <t>IT1-11 TC3</t>
-  </si>
-  <si>
-    <t>IT1-11 TC4</t>
+    <t xml:space="preserve"> Validate that appropriate error messages are displayed when required fields are left blank.</t>
+  </si>
+  <si>
+    <t>Nothing is displayed</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Add validation in the API</t>
   </si>
   <si>
     <t>IT1-12</t>
@@ -304,20 +385,38 @@
     <t>IT1-12 TC1</t>
   </si>
   <si>
+    <t>Successful Admin Update</t>
+  </si>
+  <si>
+    <t>Verify that the selected admin's information is successfully updated with valid input.</t>
+  </si>
+  <si>
     <t>IT1-12 TC2</t>
   </si>
   <si>
-    <t>IT1-12 TC3</t>
-  </si>
-  <si>
-    <t>IT1-12 TC4</t>
+    <t>error messages are displayed when required fields are left blank.</t>
+  </si>
+  <si>
+    <t>IT1-13</t>
+  </si>
+  <si>
+    <t>Add report</t>
+  </si>
+  <si>
+    <t>Successfully created a report</t>
+  </si>
+  <si>
+    <t>Verify that a report for a product is generated when a non-logged in user selects that product</t>
+  </si>
+  <si>
+    <t>Report for a product is generated when a non-logged in user selects that product</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -343,10 +442,6 @@
       <name val="Arial"/>
     </font>
     <font/>
-    <font>
-      <color rgb="FF1A1A1A"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -449,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -471,11 +566,11 @@
     <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -484,16 +579,28 @@
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
@@ -503,8 +610,20 @@
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -518,12 +637,12 @@
     <xf borderId="1" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
@@ -531,55 +650,43 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="5" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="5" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -852,850 +959,719 @@
       <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="H3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="8"/>
     </row>
     <row r="4">
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="12"/>
+      <c r="I4" s="14"/>
     </row>
     <row r="5">
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
       <c r="D5" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="13"/>
+        <v>21</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="17"/>
     </row>
     <row r="6">
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="12"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="7">
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="B7" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="22"/>
     </row>
     <row r="8">
-      <c r="B8" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>24</v>
-      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="18"/>
+        <v>29</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="17"/>
     </row>
     <row r="9">
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="13"/>
+        <v>33</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="14"/>
     </row>
     <row r="10">
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
       <c r="D10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="12"/>
+        <v>37</v>
+      </c>
+      <c r="E10" s="25"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="17"/>
     </row>
     <row r="11">
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="13"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="12">
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="B12" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="8"/>
     </row>
     <row r="13">
-      <c r="B13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="7"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="1"/>
     </row>
     <row r="14">
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
+      <c r="B14" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>46</v>
+      </c>
       <c r="D14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="12"/>
+        <v>47</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="30"/>
     </row>
     <row r="15">
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="13"/>
+        <v>51</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="8"/>
     </row>
     <row r="16">
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
       <c r="D16" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="12"/>
+        <v>55</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="31"/>
     </row>
     <row r="17">
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
       <c r="I17" s="1"/>
     </row>
     <row r="18">
-      <c r="B18" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>36</v>
+      <c r="B18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" s="22"/>
+        <v>61</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="8"/>
     </row>
     <row r="19">
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" s="7"/>
+        <v>65</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="34"/>
     </row>
     <row r="20">
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I20" s="23"/>
+        <v>69</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="35"/>
     </row>
     <row r="21">
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I21" s="7"/>
+        <v>73</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="34"/>
     </row>
     <row r="22">
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H22" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="35"/>
     </row>
     <row r="23">
-      <c r="B23" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G23" s="7"/>
-      <c r="H23" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" s="7"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="1"/>
     </row>
     <row r="24">
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G24" s="26"/>
-      <c r="H24" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I24" s="26"/>
+      <c r="B24" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" s="40"/>
     </row>
     <row r="25">
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G25" s="27"/>
-      <c r="H25" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I25" s="27"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="1"/>
     </row>
     <row r="26">
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="G26" s="26"/>
-      <c r="H26" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I26" s="26"/>
+      <c r="B26" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="8"/>
     </row>
     <row r="27">
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G27" s="27"/>
-      <c r="H27" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="I27" s="27"/>
-    </row>
-    <row r="28">
-      <c r="E28" s="29"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" ht="39.0" customHeight="1">
+      <c r="B28" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" s="43"/>
     </row>
     <row r="29">
-      <c r="B29" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I29" s="33"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="1"/>
     </row>
     <row r="30">
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I30" s="35"/>
+      <c r="B30" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" s="8"/>
     </row>
     <row r="31">
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I31" s="37"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="1"/>
     </row>
     <row r="32">
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I32" s="35"/>
+      <c r="B32" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" s="46"/>
     </row>
     <row r="33">
-      <c r="E33" s="29"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="18"/>
     </row>
     <row r="34">
       <c r="B34" s="4" t="s">
-        <v>64</v>
+        <v>110</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I34" s="7"/>
+        <v>111</v>
+      </c>
+      <c r="D34" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" s="8"/>
     </row>
     <row r="35">
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="E35" s="21"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I35" s="12"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="I35" s="35" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="36">
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I36" s="13"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="1"/>
     </row>
     <row r="37">
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I37" s="12"/>
+      <c r="B37" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F37" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I37" s="46"/>
     </row>
     <row r="38">
-      <c r="E38" s="29"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-    </row>
-    <row r="39" ht="39.0" customHeight="1">
-      <c r="B39" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="D39" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="40"/>
-      <c r="H39" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I39" s="40"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F38" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="G38" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I38" s="14"/>
+    </row>
+    <row r="39">
+      <c r="E39" s="1"/>
+      <c r="G39" s="44"/>
     </row>
     <row r="40">
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="E40" s="21"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I40" s="12"/>
+      <c r="B40" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="D40" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I40" s="8"/>
     </row>
     <row r="41">
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="41"/>
-      <c r="H41" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I41" s="41"/>
+      <c r="E41" s="1"/>
     </row>
     <row r="42">
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="E42" s="21"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I42" s="42"/>
+      <c r="E42" s="1"/>
     </row>
     <row r="43">
-      <c r="E43" s="29"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
+      <c r="E43" s="1"/>
     </row>
     <row r="44">
-      <c r="B44" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D44" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I44" s="7"/>
+      <c r="E44" s="1"/>
     </row>
     <row r="45">
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I45" s="12"/>
+      <c r="E45" s="1"/>
     </row>
     <row r="46">
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="E46" s="6"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I46" s="13"/>
+      <c r="E46" s="1"/>
     </row>
     <row r="47">
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I47" s="12"/>
+      <c r="E47" s="1"/>
     </row>
     <row r="48">
-      <c r="E48" s="29"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
+      <c r="E48" s="1"/>
     </row>
     <row r="49">
-      <c r="B49" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C49" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="D49" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="E49" s="6"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="44"/>
-      <c r="H49" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I49" s="44"/>
+      <c r="E49" s="1"/>
     </row>
     <row r="50">
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="E50" s="11"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I50" s="12"/>
+      <c r="E50" s="1"/>
     </row>
     <row r="51">
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="31" t="s">
-        <v>86</v>
-      </c>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I51" s="13"/>
+      <c r="E51" s="1"/>
     </row>
     <row r="52">
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I52" s="12"/>
+      <c r="E52" s="1"/>
     </row>
     <row r="53">
-      <c r="E53" s="29"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="1"/>
+      <c r="E53" s="1"/>
     </row>
     <row r="54">
-      <c r="B54" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D54" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I54" s="7"/>
+      <c r="E54" s="1"/>
     </row>
     <row r="55">
-      <c r="B55" s="9"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I55" s="12"/>
+      <c r="E55" s="1"/>
     </row>
     <row r="56">
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="E56" s="6"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I56" s="13"/>
+      <c r="E56" s="1"/>
     </row>
     <row r="57">
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="12"/>
-      <c r="H57" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I57" s="12"/>
+      <c r="E57" s="1"/>
     </row>
     <row r="58">
-      <c r="E58" s="29"/>
-      <c r="F58" s="15"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
+      <c r="E58" s="1"/>
     </row>
     <row r="59">
-      <c r="B59" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="C59" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="D59" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="E59" s="6"/>
-      <c r="F59" s="32"/>
-      <c r="G59" s="44"/>
-      <c r="H59" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I59" s="44"/>
+      <c r="E59" s="1"/>
     </row>
     <row r="60">
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="E60" s="11"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I60" s="12"/>
+      <c r="E60" s="1"/>
     </row>
     <row r="61">
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="E61" s="36"/>
-      <c r="F61" s="36"/>
-      <c r="G61" s="13"/>
-      <c r="H61" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I61" s="13"/>
+      <c r="E61" s="1"/>
     </row>
     <row r="62">
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
-      <c r="G62" s="12"/>
-      <c r="H62" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I62" s="12"/>
+      <c r="E62" s="1"/>
     </row>
     <row r="63">
       <c r="E63" s="1"/>
-      <c r="G63" s="1"/>
     </row>
     <row r="64">
       <c r="E64" s="1"/>
-      <c r="G64" s="1"/>
     </row>
     <row r="65">
       <c r="E65" s="1"/>
-      <c r="G65" s="1"/>
     </row>
     <row r="66">
       <c r="E66" s="1"/>
-      <c r="G66" s="1"/>
     </row>
     <row r="67">
       <c r="E67" s="1"/>
@@ -4274,116 +4250,23 @@
     <row r="925">
       <c r="E925" s="1"/>
     </row>
-    <row r="926">
-      <c r="E926" s="1"/>
-    </row>
-    <row r="927">
-      <c r="E927" s="1"/>
-    </row>
-    <row r="928">
-      <c r="E928" s="1"/>
-    </row>
-    <row r="929">
-      <c r="E929" s="1"/>
-    </row>
-    <row r="930">
-      <c r="E930" s="1"/>
-    </row>
-    <row r="931">
-      <c r="E931" s="1"/>
-    </row>
-    <row r="932">
-      <c r="E932" s="1"/>
-    </row>
-    <row r="933">
-      <c r="E933" s="1"/>
-    </row>
-    <row r="934">
-      <c r="E934" s="1"/>
-    </row>
-    <row r="935">
-      <c r="E935" s="1"/>
-    </row>
-    <row r="936">
-      <c r="E936" s="1"/>
-    </row>
-    <row r="937">
-      <c r="E937" s="1"/>
-    </row>
-    <row r="938">
-      <c r="E938" s="1"/>
-    </row>
-    <row r="939">
-      <c r="E939" s="1"/>
-    </row>
-    <row r="940">
-      <c r="E940" s="1"/>
-    </row>
-    <row r="941">
-      <c r="E941" s="1"/>
-    </row>
-    <row r="942">
-      <c r="E942" s="1"/>
-    </row>
-    <row r="943">
-      <c r="E943" s="1"/>
-    </row>
-    <row r="944">
-      <c r="E944" s="1"/>
-    </row>
-    <row r="945">
-      <c r="E945" s="1"/>
-    </row>
-    <row r="946">
-      <c r="E946" s="1"/>
-    </row>
-    <row r="947">
-      <c r="E947" s="1"/>
-    </row>
-    <row r="948">
-      <c r="E948" s="1"/>
-    </row>
-    <row r="949">
-      <c r="E949" s="1"/>
-    </row>
-    <row r="950">
-      <c r="E950" s="1"/>
-    </row>
-    <row r="951">
-      <c r="E951" s="1"/>
-    </row>
-    <row r="952">
-      <c r="E952" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="C59:C62"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="C49:C52"/>
-    <mergeCell ref="C54:C57"/>
+  <mergeCells count="12">
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C18:C22"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="H3:H6 H8:H11 H13:H16 H18:H21 H23:H27 H29:H32 H34:H37 H39:H42 H44:H47 H49:H52 H54:H57 H59:H62">
+    <dataValidation type="list" allowBlank="1" sqref="H3:H5 H7:H10 H12 H14:H16 H18:H22 H24 H26 H28 H30 H32 H34:H35 H37:H38 H40">
       <formula1>"Passed,Failed,N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>